<commit_message>
Required Fields FE + BE and Snackbar Handling of Errors
</commit_message>
<xml_diff>
--- a/src2/test.xlsx
+++ b/src2/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hanna\dev\workspace\chromeQuotes\src2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DAE204-4398-475B-ADF1-F0C32BD25F84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C90C0B-2BE0-481C-AB84-2E12FFA178AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9060" xr2:uid="{F1B0B200-413A-41FD-8560-2BCC6F80804C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
   <si>
     <t>quote</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>SuperZitat 2</t>
-  </si>
-  <si>
-    <t>SuperZitat 3</t>
   </si>
   <si>
     <t>SuperZitat 4</t>
@@ -465,7 +462,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,9 +510,6 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -528,7 +522,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -542,7 +536,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -556,7 +550,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -570,7 +564,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -584,7 +578,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -598,7 +592,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -612,7 +606,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -626,7 +620,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -640,7 +634,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -654,7 +648,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -668,7 +662,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -682,7 +676,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -696,7 +690,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
@@ -710,7 +704,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
@@ -724,7 +718,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -738,7 +732,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
@@ -752,7 +746,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Zwischenstand Code aufräumen + Run Icon
</commit_message>
<xml_diff>
--- a/src2/test.xlsx
+++ b/src2/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hanna\dev\workspace\chromeQuotes\src2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C90C0B-2BE0-481C-AB84-2E12FFA178AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0877BF-2D0F-4879-BBB1-347202CDC475}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9060" xr2:uid="{F1B0B200-413A-41FD-8560-2BCC6F80804C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
   <si>
     <t>quote</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>SuperZitat 20</t>
+  </si>
+  <si>
+    <t>SuperZitat 3</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,6 +513,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Adding Scss and using Mat variables
</commit_message>
<xml_diff>
--- a/src2/test.xlsx
+++ b/src2/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hanna\dev\workspace\chromeQuotes\src2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07347B6F-69FC-457B-981A-376506E4EAF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78AE292-E991-43B9-8837-E4A84586AC2B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9060" xr2:uid="{F1B0B200-413A-41FD-8560-2BCC6F80804C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>quote</t>
   </si>
@@ -66,13 +66,40 @@
   </si>
   <si>
     <t>Bildung, Respekt</t>
+  </si>
+  <si>
+    <t>Nathaniel Branden</t>
+  </si>
+  <si>
+    <t>La vera autostima è quella che proviamo per noi stessi quando qualcosa va storto.</t>
+  </si>
+  <si>
+    <t>Selbstwert</t>
+  </si>
+  <si>
+    <t>Denis Waitley</t>
+  </si>
+  <si>
+    <t>Quando sei capace di applaudire te stesso, è molto più facile applaudire gli altri.</t>
+  </si>
+  <si>
+    <t>Selbstwert, Italienisch</t>
+  </si>
+  <si>
+    <t>You never change things by fighting the existing reality. To change something, build a new model that makes the existing model obsolete</t>
+  </si>
+  <si>
+    <t>Buckminster Fuller</t>
+  </si>
+  <si>
+    <t>Transformation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +110,19 @@
     <font>
       <sz val="8"/>
       <color rgb="FF8B4016"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -107,10 +147,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -425,13 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113B2B80-2DE7-4C43-801D-A11BC70879F6}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -481,6 +526,39 @@
       </c>
       <c r="D4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>